<commit_message>
Fix relative F2 calculation
</commit_message>
<xml_diff>
--- a/results/analysis/analysis.xlsx
+++ b/results/analysis/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365.sharepoint.com/sites/SOLSTICIAUPM/Documentos compartidos/General/Paper IEEE Access/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{022F7976-E9A3-4265-9714-9A592995E4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{226751AE-E17D-478A-8952-444DF3AD3EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9104,49 +9104,49 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.96222064561901377</c:v>
+                  <c:v>1.0145876192257337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78947368421052633</c:v>
+                  <c:v>0.69364161849710992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85563161169881774</c:v>
+                  <c:v>0.76050884955752218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76438210227272718</c:v>
+                  <c:v>1.1417583874817661</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.49698795180722893</c:v>
+                  <c:v>0.3923900118906064</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76411960132890355</c:v>
+                  <c:v>0.68862275449101795</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63192904656319282</c:v>
+                  <c:v>0.63298167684619655</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63829787234042556</c:v>
+                  <c:v>0.44117647058823523</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.66455696202531644</c:v>
+                  <c:v>0.53299492385786795</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.74514038876889854</c:v>
+                  <c:v>0.63071297989031072</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.67092651757188493</c:v>
+                  <c:v>0.44491525423728806</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.57471264367816077</c:v>
+                  <c:v>0.43290043290043284</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.74437030859049214</c:v>
+                  <c:v>0.60263335584064825</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.59234507897934396</c:v>
+                  <c:v>0.46450690805145306</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63531353135313529</c:v>
+                  <c:v>0.41001064962726302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9243,49 +9243,49 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.9831460674157303</c:v>
+                  <c:v>1.1146496815286624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82191780821917793</c:v>
+                  <c:v>0.80536912751677847</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88028169014084501</c:v>
+                  <c:v>0.84459459459459441</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76642335766423353</c:v>
+                  <c:v>1.1602209944751383</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.58823529411764708</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.78767123287671226</c:v>
+                  <c:v>0.77181208053691264</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.65934065934065933</c:v>
+                  <c:v>0.759493670886076</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68181818181818177</c:v>
+                  <c:v>0.5357142857142857</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71917808219178092</c:v>
+                  <c:v>0.7046979865771813</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.78767123287671226</c:v>
+                  <c:v>0.77181208053691264</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.78358208955223885</c:v>
+                  <c:v>0.71917808219178081</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.64935064935064934</c:v>
+                  <c:v>0.66225165562913912</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.78358208955223885</c:v>
+                  <c:v>0.71917808219178081</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.61475409836065575</c:v>
+                  <c:v>0.52447552447552448</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.68627450980392157</c:v>
+                  <c:v>0.50724637681159424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19149,8 +19149,8 @@
   <dimension ref="A1:AA77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20596,11 +20596,11 @@
         <v>0.4</v>
       </c>
       <c r="C25" s="25">
-        <f t="shared" ref="C25:Q25" si="13">C20/(C20+C19)</f>
+        <f>C20/(C20+C19)</f>
         <v>0.46666666666666667</v>
       </c>
       <c r="D25" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="C25:Q25" si="13">D20/(D20+D19)</f>
         <v>0.32</v>
       </c>
       <c r="E25" s="25">
@@ -21144,68 +21144,68 @@
         <v>81</v>
       </c>
       <c r="B34" s="26">
-        <f>(1+2^2)*B27*B26/(2^2*B27+B26)</f>
+        <f>(1+2^2)*B26*B27/(2^2*B26+B27)</f>
         <v>1</v>
       </c>
       <c r="C34" s="26">
-        <f t="shared" ref="C34:Q34" si="15">(1+2^2)*C27*C26/(2^2*C27+C26)</f>
-        <v>0.96222064561901377</v>
+        <f t="shared" ref="C34:Q34" si="15">(1+2^2)*C26*C27/(2^2*C26+C27)</f>
+        <v>1.0145876192257337</v>
       </c>
       <c r="D34" s="26">
         <f t="shared" si="15"/>
-        <v>0.78947368421052633</v>
+        <v>0.69364161849710992</v>
       </c>
       <c r="E34" s="26">
         <f t="shared" si="15"/>
-        <v>0.85563161169881774</v>
+        <v>0.76050884955752218</v>
       </c>
       <c r="F34" s="26">
         <f t="shared" si="15"/>
-        <v>0.76438210227272718</v>
+        <v>1.1417583874817661</v>
       </c>
       <c r="G34" s="26">
         <f t="shared" si="15"/>
-        <v>0.49698795180722893</v>
+        <v>0.3923900118906064</v>
       </c>
       <c r="H34" s="26">
         <f t="shared" si="15"/>
-        <v>0.76411960132890355</v>
+        <v>0.68862275449101795</v>
       </c>
       <c r="I34" s="26">
         <f t="shared" si="15"/>
-        <v>0.63192904656319282</v>
+        <v>0.63298167684619655</v>
       </c>
       <c r="J34" s="26">
         <f t="shared" si="15"/>
-        <v>0.63829787234042556</v>
+        <v>0.44117647058823523</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="15"/>
-        <v>0.66455696202531644</v>
+        <v>0.53299492385786795</v>
       </c>
       <c r="L34" s="26">
         <f t="shared" si="15"/>
-        <v>0.74514038876889854</v>
+        <v>0.63071297989031072</v>
       </c>
       <c r="M34" s="26">
         <f t="shared" si="15"/>
-        <v>0.67092651757188493</v>
+        <v>0.44491525423728806</v>
       </c>
       <c r="N34" s="26">
         <f t="shared" si="15"/>
-        <v>0.57471264367816077</v>
+        <v>0.43290043290043284</v>
       </c>
       <c r="O34" s="26">
         <f t="shared" si="15"/>
-        <v>0.74437030859049214</v>
+        <v>0.60263335584064825</v>
       </c>
       <c r="P34" s="26">
         <f t="shared" si="15"/>
-        <v>0.59234507897934396</v>
+        <v>0.46450690805145306</v>
       </c>
       <c r="Q34" s="26">
         <f t="shared" si="15"/>
-        <v>0.63531353135313529</v>
+        <v>0.41001064962726302</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="14.45">
@@ -21213,68 +21213,68 @@
         <v>82</v>
       </c>
       <c r="B35" s="26">
-        <f t="shared" ref="B35:Q35" si="16">(1+2^2)*B28*B26/(2^2*B28+B26)</f>
+        <f>(1+2^2)*B26*B28/(2^2*B26+B28)</f>
         <v>1</v>
       </c>
       <c r="C35" s="26">
-        <f t="shared" si="16"/>
-        <v>0.9831460674157303</v>
+        <f t="shared" ref="C35:Q35" si="16">(1+2^2)*C26*C28/(2^2*C26+C28)</f>
+        <v>1.1146496815286624</v>
       </c>
       <c r="D35" s="26">
         <f t="shared" si="16"/>
-        <v>0.82191780821917793</v>
+        <v>0.80536912751677847</v>
       </c>
       <c r="E35" s="26">
         <f t="shared" si="16"/>
-        <v>0.88028169014084501</v>
+        <v>0.84459459459459441</v>
       </c>
       <c r="F35" s="26">
         <f t="shared" si="16"/>
-        <v>0.76642335766423353</v>
+        <v>1.1602209944751383</v>
       </c>
       <c r="G35" s="26">
         <f t="shared" si="16"/>
-        <v>0.55555555555555558</v>
+        <v>0.58823529411764708</v>
       </c>
       <c r="H35" s="26">
         <f t="shared" si="16"/>
-        <v>0.78767123287671226</v>
+        <v>0.77181208053691264</v>
       </c>
       <c r="I35" s="26">
         <f t="shared" si="16"/>
-        <v>0.65934065934065933</v>
+        <v>0.759493670886076</v>
       </c>
       <c r="J35" s="26">
         <f t="shared" si="16"/>
-        <v>0.68181818181818177</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="K35" s="26">
         <f t="shared" si="16"/>
-        <v>0.71917808219178092</v>
+        <v>0.7046979865771813</v>
       </c>
       <c r="L35" s="26">
         <f t="shared" si="16"/>
-        <v>0.78767123287671226</v>
+        <v>0.77181208053691264</v>
       </c>
       <c r="M35" s="26">
         <f t="shared" si="16"/>
-        <v>0.78358208955223885</v>
+        <v>0.71917808219178081</v>
       </c>
       <c r="N35" s="26">
         <f t="shared" si="16"/>
-        <v>0.64935064935064934</v>
+        <v>0.66225165562913912</v>
       </c>
       <c r="O35" s="26">
         <f t="shared" si="16"/>
-        <v>0.78358208955223885</v>
+        <v>0.71917808219178081</v>
       </c>
       <c r="P35" s="26">
         <f t="shared" si="16"/>
-        <v>0.61475409836065575</v>
+        <v>0.52447552447552448</v>
       </c>
       <c r="Q35" s="26">
         <f t="shared" si="16"/>
-        <v>0.68627450980392157</v>
+        <v>0.50724637681159424</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="14.45">
@@ -23495,7 +23495,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E1" activeCellId="1" sqref="B1:B1048576 E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24316,7 +24316,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35483,8 +35483,8 @@
   <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AC17" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ32" sqref="AJ32"/>
+      <pane xSplit="3" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AK1" activeCellId="2" sqref="B1:B1048576 AJ1:AJ1048576 AK1:AK1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>

</xml_diff>